<commit_message>
modify input for setting
</commit_message>
<xml_diff>
--- a/sw/doc/main_input.xlsx
+++ b/sw/doc/main_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baoshi/Proj/VGMPlayer/sw/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proj-Git\VGMPlayer\sw\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328FDBD5-49CD-8C4D-8A40-DED514410A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240BB8CB-D396-41FD-995E-1146112B8E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{2C1EBD94-2A85-492A-A01D-62985E686E7E}"/>
+    <workbookView xWindow="3936" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{2C1EBD94-2A85-492A-A01D-62985E686E7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>State</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Alert</t>
+  </si>
+  <si>
+    <t>Popups</t>
   </si>
 </sst>
 </file>
@@ -493,20 +496,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920A25B8-5F56-41F6-9898-B28A8FA848D3}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -536,7 +539,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -556,7 +559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -570,35 +573,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -612,27 +587,63 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto advance in player
</commit_message>
<xml_diff>
--- a/sw/doc/main_input.xlsx
+++ b/sw/doc/main_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proj-Git\VGMPlayer\sw\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baoshi/Proj/VGMPlayer/sw/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240BB8CB-D396-41FD-995E-1146112B8E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6698FB-8D76-C647-8895-BB0E7BFC5A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3936" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{2C1EBD94-2A85-492A-A01D-62985E686E7E}"/>
+    <workbookView xWindow="-30820" yWindow="4820" windowWidth="23260" windowHeight="12460" xr2:uid="{2C1EBD94-2A85-492A-A01D-62985E686E7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>State</t>
   </si>
@@ -107,12 +107,6 @@
     <t>Player_S16</t>
   </si>
   <si>
-    <t>Player_S16_Playing</t>
-  </si>
-  <si>
-    <t>Player_S16_Paused</t>
-  </si>
-  <si>
     <t>Button (LV_EVENT_SHORT_CLICKED)
 EVT_BUTTON_PLAY_CLICKED</t>
   </si>
@@ -121,6 +115,17 @@
   </si>
   <si>
     <t>Popups</t>
+  </si>
+  <si>
+    <t>Button (LV_EVENT_SHORT_CLICKED)
+EVT_BUTTON_UP_CLICKED</t>
+  </si>
+  <si>
+    <t>Button (LV_EVENT_SHORT_CLICKED)
+EVT_BUTTON_DOWN_CLICKED</t>
+  </si>
+  <si>
+    <t>∂</t>
   </si>
 </sst>
 </file>
@@ -162,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -181,6 +186,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,18 +506,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920A25B8-5F56-41F6-9898-B28A8FA848D3}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -539,7 +547,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -559,7 +567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -573,7 +581,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -584,47 +592,66 @@
         <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -641,7 +668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Add power off function
</commit_message>
<xml_diff>
--- a/sw/doc/main_input.xlsx
+++ b/sw/doc/main_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proj-Git\VGMPlayer\sw\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baoshi/Proj/VGMPlayer/sw/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960EF629-7896-458C-A153-38EA4F64CEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9210D586-835F-C849-A181-4367847F18D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3936" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{2C1EBD94-2A85-492A-A01D-62985E686E7E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" xr2:uid="{2C1EBD94-2A85-492A-A01D-62985E686E7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>State</t>
   </si>
@@ -136,6 +136,9 @@
   <si>
     <t>Button (LV_EVENT_SHORT_CLICKED)
 EVT_CLOSE_VOLUME_POPUP</t>
+  </si>
+  <si>
+    <t>Button (LV_EVENT_LONG_PRESSED) EVT_BUTTON_BACK_LONG_PRESSED</t>
   </si>
 </sst>
 </file>
@@ -200,10 +203,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -238,8 +241,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6B89480-80F6-466A-8843-92CCD69D0E9E}" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="0">
-  <autoFilter ref="A1:F10" xr:uid="{F6B89480-80F6-466A-8843-92CCD69D0E9E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6B89480-80F6-466A-8843-92CCD69D0E9E}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F13" xr:uid="{F6B89480-80F6-466A-8843-92CCD69D0E9E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -248,12 +251,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{122113DE-2ABA-4892-8D08-6E5458E75A48}" name="State" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{68A369B7-A83F-4F84-9E49-C8504BFF2E0D}" name="INPUT_KEY_SETTING" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{7F38BB4B-2031-44FF-A15D-503D6D0092B1}" name="INPUT_KEY_BACK" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{78BC94CB-F7CE-4EAA-B87B-2DAD39F8CB81}" name="INPUT_KEY_PLAY" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{404120CC-0AEC-4A37-AFAD-19A019BF3174}" name="INPUT_KEY_UP" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4322BB19-4EEC-4A23-9765-6DFF3DE70817}" name="INPUT_KEY_DOWN" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{122113DE-2ABA-4892-8D08-6E5458E75A48}" name="State" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{68A369B7-A83F-4F84-9E49-C8504BFF2E0D}" name="INPUT_KEY_SETTING" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{7F38BB4B-2031-44FF-A15D-503D6D0092B1}" name="INPUT_KEY_BACK" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{78BC94CB-F7CE-4EAA-B87B-2DAD39F8CB81}" name="INPUT_KEY_PLAY" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{404120CC-0AEC-4A37-AFAD-19A019BF3174}" name="INPUT_KEY_UP" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{4322BB19-4EEC-4A23-9765-6DFF3DE70817}" name="INPUT_KEY_DOWN" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -556,20 +559,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920A25B8-5F56-41F6-9898-B28A8FA848D3}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,14 +592,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -616,20 +619,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>20</v>
@@ -638,89 +639,112 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>